<commit_message>
Added ribbon cables to parts list
</commit_message>
<xml_diff>
--- a/logistics/plattonPartsList.xlsx
+++ b/logistics/plattonPartsList.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="86">
   <si>
     <t>Raspberry Pi</t>
   </si>
@@ -270,6 +270,15 @@
   </si>
   <si>
     <t>Newegg</t>
+  </si>
+  <si>
+    <t>10Wire Ribbon cable</t>
+  </si>
+  <si>
+    <t>Cabling for Range Sensor and LCD</t>
+  </si>
+  <si>
+    <t>CAB-10647</t>
   </si>
 </sst>
 </file>
@@ -435,7 +444,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -500,6 +509,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -802,10 +814,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J44"/>
+  <dimension ref="A2:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -997,7 +1009,7 @@
         <v>20.329999999999998</v>
       </c>
       <c r="I7" s="19">
-        <f t="shared" ref="I7:I18" si="1">G7*H7</f>
+        <f t="shared" ref="I7:I19" si="1">G7*H7</f>
         <v>20.329999999999998</v>
       </c>
       <c r="J7" s="18" t="s">
@@ -1236,40 +1248,41 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
+        <v>83</v>
+      </c>
+      <c r="B16" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="38" t="s">
+        <v>85</v>
+      </c>
       <c r="E16" s="17"/>
       <c r="F16" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" s="18">
-        <v>1</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="G16" s="18"/>
       <c r="H16" s="19"/>
-      <c r="I16" s="19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J16" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I16" s="19"/>
+      <c r="J16" s="20"/>
+    </row>
+    <row r="17" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="17"/>
+        <v>11</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>14</v>
+      </c>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
+      <c r="F17" s="17" t="s">
+        <v>13</v>
+      </c>
       <c r="G17" s="18">
         <v>1</v>
       </c>
@@ -1284,7 +1297,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
@@ -1304,166 +1317,160 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="18"/>
+      <c r="A19" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="18">
+        <v>1</v>
+      </c>
       <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
+      <c r="I19" s="19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="J19" s="18" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="9" t="s">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="G20" s="10"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11">
-        <f>SUM(I3:I18)</f>
+      <c r="G21" s="10"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11">
+        <f>SUM(I3:I19)</f>
         <v>138.52759999999998</v>
       </c>
-      <c r="J20" s="3"/>
-    </row>
-    <row r="21" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="6"/>
-      <c r="B21" s="29" t="s">
+      <c r="J21" s="3"/>
+    </row>
+    <row r="22" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="6"/>
+      <c r="B22" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="C21" s="12">
+      <c r="C22" s="12">
         <v>227.22</v>
       </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="16" t="s">
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="I24" s="1"/>
-    </row>
-    <row r="26" spans="1:10" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="30" t="s">
+      <c r="I25" s="1"/>
+    </row>
+    <row r="27" spans="1:10" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="31" t="s">
+      <c r="B27" s="31" t="s">
         <v>27</v>
-      </c>
-      <c r="C26" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="D26" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="E26" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="F26" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="G26" s="31">
-        <v>6</v>
-      </c>
-      <c r="H26" s="33">
-        <v>35</v>
-      </c>
-      <c r="I26" s="33">
-        <f t="shared" ref="I26:I32" si="2">G26*H26</f>
-        <v>210</v>
-      </c>
-      <c r="J26" s="35" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27" s="31">
-        <v>801</v>
       </c>
       <c r="C27" s="31" t="s">
         <v>74</v>
       </c>
       <c r="D27" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="E27" s="31"/>
+        <v>28</v>
+      </c>
+      <c r="E27" s="31" t="s">
+        <v>3</v>
+      </c>
       <c r="F27" s="30" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="G27" s="31">
         <v>6</v>
       </c>
       <c r="H27" s="33">
+        <v>35</v>
+      </c>
+      <c r="I27" s="33">
+        <f t="shared" ref="I27:I33" si="2">G27*H27</f>
+        <v>210</v>
+      </c>
+      <c r="J27" s="35" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="31">
+        <v>801</v>
+      </c>
+      <c r="C28" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28" s="31"/>
+      <c r="F28" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" s="31">
+        <v>6</v>
+      </c>
+      <c r="H28" s="33">
         <v>15.95</v>
       </c>
-      <c r="I27" s="33">
+      <c r="I28" s="33">
         <f t="shared" si="2"/>
         <v>95.699999999999989</v>
       </c>
-      <c r="J27" s="34" t="s">
+      <c r="J28" s="34" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="C28" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="G28" s="27">
-        <v>6</v>
-      </c>
-      <c r="H28" s="28">
-        <v>0</v>
-      </c>
-      <c r="I28" s="28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J28" s="26" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A29" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" s="27"/>
+        <v>31</v>
+      </c>
+      <c r="B29" s="27" t="s">
+        <v>30</v>
+      </c>
       <c r="C29" s="27" t="s">
         <v>54</v>
       </c>
       <c r="D29" s="27"/>
       <c r="E29" s="27"/>
       <c r="F29" s="26" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G29" s="27">
         <v>6</v>
@@ -1475,219 +1482,246 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J29" s="27"/>
-    </row>
-    <row r="30" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A30" s="30" t="s">
+      <c r="J29" s="26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="G30" s="27">
+        <v>6</v>
+      </c>
+      <c r="H30" s="28">
+        <v>0</v>
+      </c>
+      <c r="I30" s="28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J30" s="27"/>
+    </row>
+    <row r="31" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A31" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31" t="s">
+      <c r="B31" s="31"/>
+      <c r="C31" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="D30" s="32" t="s">
+      <c r="D31" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="E30" s="31"/>
-      <c r="F30" s="30" t="s">
+      <c r="E31" s="31"/>
+      <c r="F31" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="G30" s="31">
+      <c r="G31" s="31">
         <v>36</v>
       </c>
-      <c r="H30" s="33">
+      <c r="H31" s="33">
         <v>0.50760000000000005</v>
       </c>
-      <c r="I30" s="33">
+      <c r="I31" s="33">
         <f t="shared" si="2"/>
         <v>18.273600000000002</v>
       </c>
-      <c r="J30" s="34" t="s">
+      <c r="J31" s="34" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="30" t="s">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="31" t="s">
+      <c r="B32" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="C31" s="31" t="s">
+      <c r="C32" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D31" s="32" t="s">
+      <c r="D32" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="E31" s="31"/>
-      <c r="F31" s="30" t="s">
+      <c r="E32" s="31"/>
+      <c r="F32" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="G31" s="31">
+      <c r="G32" s="31">
         <v>6</v>
       </c>
-      <c r="H31" s="33">
+      <c r="H32" s="33">
         <v>25.95</v>
       </c>
-      <c r="I31" s="33">
+      <c r="I32" s="33">
         <f t="shared" si="2"/>
         <v>155.69999999999999</v>
       </c>
-      <c r="J31" s="34" t="s">
+      <c r="J32" s="34" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="30" t="s">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="B32" s="31"/>
-      <c r="C32" s="36" t="s">
+      <c r="B33" s="31"/>
+      <c r="C33" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="32" t="s">
+      <c r="D33" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="E32" s="31"/>
-      <c r="F32" s="30" t="s">
+      <c r="E33" s="31"/>
+      <c r="F33" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="G32" s="31">
+      <c r="G33" s="31">
         <v>6</v>
       </c>
-      <c r="H32" s="33">
+      <c r="H33" s="33">
         <v>9.9499999999999993</v>
       </c>
-      <c r="I32" s="33">
+      <c r="I33" s="33">
         <f t="shared" si="2"/>
         <v>59.699999999999996</v>
       </c>
-      <c r="J32" s="34" t="s">
+      <c r="J33" s="34" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="B33" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="C33" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="D33" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="E33" s="31"/>
-      <c r="F33" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="G33" s="31">
-        <v>6</v>
-      </c>
-      <c r="H33" s="33">
-        <v>15.95</v>
-      </c>
-      <c r="I33" s="33">
-        <f t="shared" ref="I33:I34" si="3">G33*H33</f>
-        <v>95.699999999999989</v>
-      </c>
-      <c r="J33" s="34" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="30" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B34" s="31" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
       <c r="C34" s="31" t="s">
         <v>44</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
       <c r="E34" s="31"/>
       <c r="F34" s="30" t="s">
-        <v>66</v>
+        <v>19</v>
       </c>
       <c r="G34" s="31">
         <v>6</v>
       </c>
       <c r="H34" s="33">
+        <v>15.95</v>
+      </c>
+      <c r="I34" s="33">
+        <f t="shared" ref="I34:I35" si="3">G34*H34</f>
+        <v>95.699999999999989</v>
+      </c>
+      <c r="J34" s="34" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="E35" s="31"/>
+      <c r="F35" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="G35" s="31">
+        <v>6</v>
+      </c>
+      <c r="H35" s="33">
         <v>0.95</v>
       </c>
-      <c r="I34" s="33">
+      <c r="I35" s="33">
         <f t="shared" si="3"/>
         <v>5.6999999999999993</v>
       </c>
-      <c r="J34" s="34" t="s">
+      <c r="J35" s="34" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="14" t="s">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="I35" s="15">
-        <f>SUM(I26:I34)</f>
+      <c r="I36" s="15">
+        <f>SUM(I27:I35)</f>
         <v>640.77359999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="F38" s="7" t="s">
+    <row r="39" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="F39" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="8">
-        <f>SUM(C21,I35)</f>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="8">
+        <f>SUM(C22,I36)</f>
         <v>867.99360000000001</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>71</v>
-      </c>
-      <c r="B41">
-        <v>28.94</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B42">
-        <v>332.03</v>
+        <v>28.94</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>81</v>
+      </c>
+      <c r="B43">
+        <v>332.03</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>82</v>
       </c>
-      <c r="B43">
+      <c r="B44">
         <f>25.48+64.44+159.3</f>
         <v>249.22000000000003</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B44" s="37">
-        <f>SUM(B40:B43)</f>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B45" s="37">
+        <f>SUM(B41:B44)</f>
         <v>610.19000000000005</v>
       </c>
     </row>
@@ -1696,13 +1730,13 @@
     <hyperlink ref="J3" r:id="rId1"/>
     <hyperlink ref="J4" r:id="rId2"/>
     <hyperlink ref="J12" r:id="rId3"/>
-    <hyperlink ref="J26" r:id="rId4" display="http://www.newark.com/jsp/search/productdetail.jsp?SKU=43W5302&amp;CMP=KNC-GPLA"/>
-    <hyperlink ref="J27" r:id="rId5"/>
-    <hyperlink ref="J31" r:id="rId6"/>
-    <hyperlink ref="J30" r:id="rId7"/>
-    <hyperlink ref="J33" r:id="rId8"/>
-    <hyperlink ref="J34" r:id="rId9"/>
-    <hyperlink ref="J32" r:id="rId10"/>
+    <hyperlink ref="J27" r:id="rId4" display="http://www.newark.com/jsp/search/productdetail.jsp?SKU=43W5302&amp;CMP=KNC-GPLA"/>
+    <hyperlink ref="J28" r:id="rId5"/>
+    <hyperlink ref="J32" r:id="rId6"/>
+    <hyperlink ref="J31" r:id="rId7"/>
+    <hyperlink ref="J34" r:id="rId8"/>
+    <hyperlink ref="J35" r:id="rId9"/>
+    <hyperlink ref="J33" r:id="rId10"/>
     <hyperlink ref="J13" r:id="rId11"/>
     <hyperlink ref="J11" r:id="rId12"/>
     <hyperlink ref="J9" r:id="rId13"/>

</xml_diff>

<commit_message>
Updated SD card to new 8GB card and updated Rpi and Arduino power supply information
</commit_message>
<xml_diff>
--- a/logistics/plattonPartsList.xlsx
+++ b/logistics/plattonPartsList.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="89">
   <si>
     <t>Raspberry Pi</t>
   </si>
@@ -157,9 +157,6 @@
   </si>
   <si>
     <t>http://www.newegg.com/Product/Product.aspx?Item=9SIA1HE0JZ2520</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DANE-ELEC 4GB Secure Digital High-Capacity (SDHC) Flash Card Model DA-SD-4096-R </t>
   </si>
   <si>
     <t>http://www.newegg.com/Product/Product.aspx?Item=9SIA1K50P03742</t>
@@ -279,6 +276,19 @@
   </si>
   <si>
     <t>CAB-10647</t>
+  </si>
+  <si>
+    <t>ebay.com</t>
+  </si>
+  <si>
+    <t>http://cgi.ebay.com/ws/eBayISAPI.dll?ViewItem&amp;item=400494532215</t>
+  </si>
+  <si>
+    <t>In: AC 100-240V 50/60Hz
+Out: DC12V - 2A</t>
+  </si>
+  <si>
+    <t>PNY 8GB Class 10 SDHC Card</t>
   </si>
 </sst>
 </file>
@@ -345,7 +355,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -379,6 +389,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -444,7 +460,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -512,6 +528,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -817,13 +835,13 @@
   <dimension ref="A2:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.140625" customWidth="1"/>
     <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" hidden="1" customWidth="1"/>
@@ -933,33 +951,33 @@
         <v>30</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
       <c r="F5" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G5" s="18">
         <v>1</v>
       </c>
-      <c r="H5" s="19">
-        <v>0</v>
-      </c>
-      <c r="I5" s="19">
+      <c r="H5" s="40">
+        <v>9.02</v>
+      </c>
+      <c r="I5" s="40">
         <f t="shared" ref="I5" si="0">G5*H5</f>
-        <v>0</v>
+        <v>9.02</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>40</v>
@@ -967,20 +985,20 @@
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
       <c r="F6" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G6" s="18">
         <v>1</v>
       </c>
-      <c r="H6" s="19">
-        <v>3.95</v>
-      </c>
-      <c r="I6" s="19">
+      <c r="H6" s="40">
+        <v>12.99</v>
+      </c>
+      <c r="I6" s="40">
         <f>G6*H6</f>
-        <v>3.95</v>
+        <v>12.99</v>
       </c>
       <c r="J6" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
@@ -994,7 +1012,7 @@
         <v>40</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E7" s="17">
         <v>22</v>
@@ -1018,7 +1036,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17" t="s">
@@ -1038,19 +1056,19 @@
         <v>0</v>
       </c>
       <c r="J8" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B9" s="17"/>
       <c r="C9" s="22" t="s">
         <v>44</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E9" s="17"/>
       <c r="F9" s="17" t="s">
@@ -1067,33 +1085,37 @@
         <v>9.9499999999999993</v>
       </c>
       <c r="J9" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="17"/>
+      <c r="B10" s="17" t="s">
+        <v>87</v>
+      </c>
       <c r="C10" s="17" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
       <c r="F10" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G10" s="18">
         <v>1</v>
       </c>
-      <c r="H10" s="19">
-        <v>0</v>
-      </c>
-      <c r="I10" s="19">
+      <c r="H10" s="40">
+        <v>6.35</v>
+      </c>
+      <c r="I10" s="40">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J10" s="18"/>
+        <v>6.35</v>
+      </c>
+      <c r="J10" s="39" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
@@ -1106,11 +1128,11 @@
         <v>44</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E11" s="17"/>
       <c r="F11" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G11" s="18">
         <v>1</v>
@@ -1123,7 +1145,7 @@
         <v>25.95</v>
       </c>
       <c r="J11" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1137,7 +1159,7 @@
         <v>40</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E12" s="17"/>
       <c r="F12" s="17" t="s">
@@ -1159,18 +1181,18 @@
     </row>
     <row r="13" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B13" s="17"/>
       <c r="C13" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E13" s="17"/>
       <c r="F13" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G13" s="18">
         <v>1</v>
@@ -1183,7 +1205,7 @@
         <v>0.50760000000000005</v>
       </c>
       <c r="J13" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1214,7 +1236,7 @@
         <v>15.95</v>
       </c>
       <c r="J14" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1222,17 +1244,17 @@
         <v>18</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>44</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E15" s="17"/>
       <c r="F15" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G15" s="18">
         <v>1</v>
@@ -1245,25 +1267,25 @@
         <v>0.95</v>
       </c>
       <c r="J15" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B16" s="38" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C16" s="17" t="s">
         <v>44</v>
       </c>
       <c r="D16" s="38" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E16" s="17"/>
       <c r="F16" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G16" s="18"/>
       <c r="H16" s="19"/>
@@ -1292,7 +1314,7 @@
         <v>0</v>
       </c>
       <c r="J17" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1313,7 +1335,7 @@
         <v>0</v>
       </c>
       <c r="J18" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1334,7 +1356,7 @@
         <v>0</v>
       </c>
       <c r="J19" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1350,7 +1372,7 @@
       <c r="H20" s="19"/>
       <c r="I20" s="19"/>
       <c r="J20" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
@@ -1360,20 +1382,20 @@
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G21" s="10"/>
       <c r="H21" s="11"/>
       <c r="I21" s="11">
         <f>SUM(I3:I19)</f>
-        <v>138.52759999999998</v>
+        <v>162.93759999999997</v>
       </c>
       <c r="J21" s="3"/>
     </row>
     <row r="22" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
       <c r="B22" s="29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C22" s="12">
         <v>227.22</v>
@@ -1389,7 +1411,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I25" s="1"/>
     </row>
@@ -1401,7 +1423,7 @@
         <v>27</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D27" s="31" t="s">
         <v>28</v>
@@ -1423,7 +1445,7 @@
         <v>210</v>
       </c>
       <c r="J27" s="35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1434,7 +1456,7 @@
         <v>801</v>
       </c>
       <c r="C28" s="31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D28" s="31" t="s">
         <v>37</v>
@@ -1465,12 +1487,12 @@
         <v>30</v>
       </c>
       <c r="C29" s="27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D29" s="27"/>
       <c r="E29" s="27"/>
       <c r="F29" s="26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G29" s="27">
         <v>6</v>
@@ -1483,7 +1505,7 @@
         <v>0</v>
       </c>
       <c r="J29" s="26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="34.5" x14ac:dyDescent="0.25">
@@ -1492,12 +1514,12 @@
       </c>
       <c r="B30" s="27"/>
       <c r="C30" s="27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D30" s="27"/>
       <c r="E30" s="27"/>
       <c r="F30" s="26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G30" s="27">
         <v>6</v>
@@ -1513,18 +1535,18 @@
     </row>
     <row r="31" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A31" s="30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B31" s="31"/>
       <c r="C31" s="31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D31" s="32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E31" s="31"/>
       <c r="F31" s="30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G31" s="31">
         <v>36</v>
@@ -1537,7 +1559,7 @@
         <v>18.273600000000002</v>
       </c>
       <c r="J31" s="34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -1551,11 +1573,11 @@
         <v>44</v>
       </c>
       <c r="D32" s="32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E32" s="31"/>
       <c r="F32" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G32" s="31">
         <v>6</v>
@@ -1568,19 +1590,19 @@
         <v>155.69999999999999</v>
       </c>
       <c r="J32" s="34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B33" s="31"/>
       <c r="C33" s="36" t="s">
         <v>44</v>
       </c>
       <c r="D33" s="32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E33" s="31"/>
       <c r="F33" s="30" t="s">
@@ -1597,7 +1619,7 @@
         <v>59.699999999999996</v>
       </c>
       <c r="J33" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -1628,7 +1650,7 @@
         <v>95.699999999999989</v>
       </c>
       <c r="J34" s="34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -1636,17 +1658,17 @@
         <v>18</v>
       </c>
       <c r="B35" s="31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C35" s="31" t="s">
         <v>44</v>
       </c>
       <c r="D35" s="31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E35" s="31"/>
       <c r="F35" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G35" s="31">
         <v>6</v>
@@ -1659,14 +1681,14 @@
         <v>5.6999999999999993</v>
       </c>
       <c r="J35" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F36" s="13"/>
       <c r="G36" s="13"/>
       <c r="H36" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I36" s="15">
         <f>SUM(I27:I35)</f>
@@ -1675,7 +1697,7 @@
     </row>
     <row r="39" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="F39" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
@@ -1686,17 +1708,17 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B42">
         <v>28.94</v>
@@ -1704,7 +1726,7 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B43">
         <v>332.03</v>
@@ -1712,7 +1734,7 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B44">
         <f>25.48+64.44+159.3</f>
@@ -1742,9 +1764,10 @@
     <hyperlink ref="J9" r:id="rId13"/>
     <hyperlink ref="J14" r:id="rId14"/>
     <hyperlink ref="J15" r:id="rId15"/>
+    <hyperlink ref="J10" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
 

</xml_diff>